<commit_message>
12 season, 15 matchday
</commit_message>
<xml_diff>
--- a/data/match_13.xlsx
+++ b/data/match_13.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\euroleague\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28F09FAA-0DF8-45A6-B4AD-E94C32A10D47}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="60">
   <si>
     <t>№</t>
   </si>
@@ -159,9 +153,6 @@
   </si>
   <si>
     <t>Муратов Игорь</t>
-  </si>
-  <si>
-    <t>11</t>
   </si>
   <si>
     <t>Еременко Владислав</t>
@@ -215,7 +206,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -571,16 +562,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -639,7 +630,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>5.5</v>
       </c>
@@ -698,12 +689,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -733,13 +724,13 @@
         <v>0</v>
       </c>
       <c r="N3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="O3">
         <v>0</v>
       </c>
       <c r="P3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -751,7 +742,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>5.5</v>
       </c>
@@ -810,12 +801,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -851,7 +842,7 @@
         <v>0</v>
       </c>
       <c r="P5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="Q5">
         <v>0</v>
@@ -863,12 +854,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>20.5</v>
       </c>
       <c r="B6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C6">
         <v>7</v>
@@ -922,18 +913,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C7">
         <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -981,12 +972,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C8">
         <v>11</v>
@@ -1040,12 +1031,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C9">
         <v>6</v>
@@ -1099,7 +1090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>5.5</v>
       </c>
@@ -1158,13 +1149,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1217,7 +1208,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>1.5</v>
       </c>
@@ -1276,7 +1267,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>1.5</v>
       </c>
@@ -1335,7 +1326,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>5.5</v>
       </c>
@@ -1394,12 +1385,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C16">
         <v>11</v>
@@ -1453,7 +1444,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>13</v>
       </c>
@@ -1512,7 +1503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>10</v>
       </c>
@@ -1571,36 +1562,36 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>26</v>
       </c>
       <c r="B19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C19">
         <v>0</v>
       </c>
       <c r="D19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E19">
         <v>0</v>
       </c>
       <c r="F19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G19">
         <v>0</v>
       </c>
       <c r="H19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I19">
         <v>0</v>
       </c>
       <c r="J19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K19">
         <v>0</v>
@@ -1612,25 +1603,25 @@
         <v>0</v>
       </c>
       <c r="N19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="O19">
         <v>0</v>
       </c>
       <c r="P19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="Q19">
         <v>0</v>
       </c>
       <c r="R19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="S19">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>13</v>
       </c>
@@ -1659,7 +1650,7 @@
         <v>0</v>
       </c>
       <c r="J20" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="K20">
         <v>0</v>
@@ -1689,12 +1680,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>16</v>
       </c>
       <c r="B21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C21">
         <v>11</v>
@@ -1748,7 +1739,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>8</v>
       </c>
@@ -1807,7 +1798,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>10</v>
       </c>
@@ -1866,7 +1857,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>13</v>
       </c>
@@ -1925,12 +1916,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>20.5</v>
       </c>
       <c r="B25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C25">
         <v>7</v>
@@ -1984,12 +1975,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>18</v>
       </c>
       <c r="B26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C26">
         <v>9</v>
@@ -2031,7 +2022,7 @@
         <v>0</v>
       </c>
       <c r="P26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="Q26">
         <v>2</v>
@@ -2043,12 +2034,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>24</v>
       </c>
       <c r="B27" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C27">
         <v>2</v>
@@ -2066,7 +2057,7 @@
         <v>0</v>
       </c>
       <c r="H27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I27">
         <v>0</v>
@@ -2102,7 +2093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>3</v>
       </c>
@@ -2162,7 +2153,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S28">
+  <sortState ref="A2:S28">
     <sortCondition ref="B1:B28"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>